<commit_message>
Add: Bundesliga datasets and files
</commit_message>
<xml_diff>
--- a/Data Files/Laliga/Laliga_Points_table_2025.xlsx
+++ b/Data Files/Laliga/Laliga_Points_table_2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2025 workspaces\Football League Standing Prediction v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2025 workspaces\13 Feb\Football-prediction\Data Files\Laliga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E3C862-DD52-452A-AB90-68A8BA8A76DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30A52BA-D5A0-4826-B948-5A6F4ACD9371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,9 @@
     <t>Real Madrid</t>
   </si>
   <si>
-    <t>Atletico Madrid</t>
-  </si>
-  <si>
     <t>Barcelona</t>
   </si>
   <si>
-    <t>Athletic Bilbao</t>
-  </si>
-  <si>
     <t>Villarreal</t>
   </si>
   <si>
@@ -55,9 +49,6 @@
     <t>Osasuna</t>
   </si>
   <si>
-    <t>Real Mallorca</t>
-  </si>
-  <si>
     <t>Real Betis</t>
   </si>
   <si>
@@ -85,9 +76,6 @@
     <t>Alaves</t>
   </si>
   <si>
-    <t>Real Valladolid</t>
-  </si>
-  <si>
     <t>Rank</t>
   </si>
   <si>
@@ -110,6 +98,18 @@
   </si>
   <si>
     <t>GD</t>
+  </si>
+  <si>
+    <t>Atlético</t>
+  </si>
+  <si>
+    <t>A Bilbao</t>
+  </si>
+  <si>
+    <t>Mallorca</t>
+  </si>
+  <si>
+    <t>Valladolid</t>
   </si>
 </sst>
 </file>
@@ -513,48 +513,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -586,12 +586,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>23</v>
@@ -618,12 +618,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>23</v>
@@ -650,12 +650,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>23</v>
@@ -682,12 +682,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>23</v>
@@ -714,12 +714,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>23</v>
@@ -746,12 +746,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>23</v>
@@ -778,12 +778,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>23</v>
@@ -810,12 +810,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>23</v>
@@ -842,12 +842,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>23</v>
@@ -874,12 +874,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>23</v>
@@ -906,12 +906,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>23</v>
@@ -938,12 +938,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>23</v>
@@ -970,12 +970,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>23</v>
@@ -1002,12 +1002,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>23</v>
@@ -1034,12 +1034,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>23</v>
@@ -1066,12 +1066,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>23</v>
@@ -1098,12 +1098,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>23</v>
@@ -1130,12 +1130,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>23</v>
@@ -1162,12 +1162,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>23</v>

</xml_diff>